<commit_message>
fix: timer countdown quiz
</commit_message>
<xml_diff>
--- a/public/Book1.xlsx
+++ b/public/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Code\Laravel\stupen_lms\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568E8DA5-390B-417F-88D0-DE1BF232D008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5821D41-9E9A-44A9-B14A-23B7B232B20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{42C8A19A-67FB-4F9C-B427-EE1B551A8B51}"/>
   </bookViews>
@@ -1019,7 +1019,7 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -1068,7 +1068,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -1085,7 +1085,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -1102,7 +1102,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -1119,7 +1119,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -1136,7 +1136,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
@@ -1153,7 +1153,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>21</v>
@@ -1170,7 +1170,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>23</v>
@@ -1187,7 +1187,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>25</v>
@@ -1204,7 +1204,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
@@ -1221,7 +1221,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>29</v>
@@ -1238,7 +1238,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>31</v>
@@ -1255,7 +1255,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>33</v>
@@ -1272,7 +1272,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>35</v>
@@ -1289,7 +1289,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>37</v>
@@ -1306,7 +1306,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>39</v>
@@ -1323,7 +1323,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>40</v>
@@ -1340,7 +1340,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>42</v>
@@ -1357,7 +1357,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>44</v>
@@ -1374,7 +1374,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>46</v>
@@ -1391,7 +1391,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>48</v>
@@ -1408,7 +1408,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>50</v>
@@ -1425,7 +1425,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>52</v>
@@ -1442,7 +1442,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>54</v>
@@ -1459,7 +1459,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>56</v>
@@ -1476,7 +1476,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>58</v>
@@ -1493,7 +1493,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>60</v>
@@ -1510,7 +1510,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>62</v>
@@ -1527,7 +1527,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>64</v>
@@ -1544,7 +1544,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>66</v>
@@ -1561,7 +1561,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>67</v>
@@ -1578,7 +1578,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>69</v>
@@ -1595,7 +1595,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>71</v>
@@ -1612,7 +1612,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>73</v>
@@ -1629,7 +1629,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>75</v>
@@ -1646,7 +1646,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>77</v>
@@ -1663,7 +1663,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>79</v>
@@ -1680,7 +1680,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>81</v>
@@ -1697,7 +1697,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>83</v>
@@ -1714,7 +1714,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>84</v>
@@ -1731,7 +1731,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>86</v>
@@ -1748,7 +1748,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>88</v>
@@ -1765,7 +1765,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>90</v>
@@ -1782,7 +1782,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>92</v>
@@ -1799,7 +1799,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>94</v>
@@ -1816,7 +1816,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>96</v>
@@ -1833,7 +1833,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>98</v>
@@ -1850,7 +1850,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>100</v>
@@ -1867,7 +1867,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>101</v>
@@ -1884,7 +1884,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>103</v>
@@ -1901,7 +1901,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>105</v>
@@ -1918,7 +1918,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>106</v>
@@ -1935,7 +1935,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>108</v>
@@ -1952,7 +1952,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>110</v>
@@ -1969,7 +1969,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>112</v>
@@ -1986,7 +1986,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>114</v>
@@ -2003,7 +2003,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>116</v>
@@ -2020,7 +2020,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>118</v>
@@ -2037,7 +2037,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>120</v>
@@ -2054,7 +2054,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>122</v>
@@ -2071,7 +2071,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>124</v>
@@ -2088,7 +2088,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>126</v>
@@ -2105,7 +2105,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>128</v>
@@ -2122,7 +2122,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>130</v>
@@ -2139,7 +2139,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>132</v>
@@ -2156,7 +2156,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>134</v>
@@ -2173,7 +2173,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>136</v>
@@ -2190,7 +2190,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>138</v>
@@ -2207,7 +2207,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>140</v>
@@ -2224,7 +2224,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>142</v>
@@ -2241,7 +2241,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>144</v>
@@ -2258,7 +2258,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>146</v>
@@ -2275,7 +2275,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>148</v>
@@ -2292,7 +2292,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>150</v>
@@ -2309,7 +2309,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>152</v>
@@ -2326,7 +2326,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>154</v>
@@ -2343,7 +2343,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>156</v>
@@ -2360,7 +2360,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>158</v>
@@ -2377,7 +2377,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>160</v>
@@ -2394,7 +2394,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>162</v>
@@ -2411,7 +2411,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>164</v>
@@ -2428,7 +2428,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>166</v>
@@ -2445,7 +2445,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>168</v>
@@ -2462,7 +2462,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>170</v>
@@ -2479,7 +2479,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>172</v>
@@ -2496,7 +2496,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>174</v>
@@ -2513,7 +2513,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>176</v>
@@ -2530,7 +2530,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>178</v>
@@ -2547,7 +2547,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>180</v>
@@ -2564,7 +2564,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>182</v>
@@ -2581,7 +2581,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>184</v>
@@ -2598,7 +2598,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>186</v>
@@ -2615,7 +2615,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>188</v>
@@ -2632,7 +2632,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>190</v>
@@ -2649,7 +2649,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>192</v>
@@ -2666,7 +2666,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>194</v>
@@ -2683,7 +2683,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>196</v>
@@ -2700,7 +2700,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>198</v>
@@ -2717,7 +2717,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>200</v>
@@ -2734,7 +2734,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>201</v>

</xml_diff>